<commit_message>
updated mutationsTable.xlsx (new variant - C.36.3.1)
</commit_message>
<xml_diff>
--- a/mutationsTable.xlsx
+++ b/mutationsTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" tabRatio="846" firstSheet="14" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" tabRatio="846" firstSheet="15" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="B.1.1.7" sheetId="13" r:id="rId1"/>
@@ -38,15 +38,16 @@
     <sheet name="VUI_P681H_Israel" sheetId="24" r:id="rId24"/>
     <sheet name="VUI_L452R|L1063F_Israel" sheetId="25" r:id="rId25"/>
     <sheet name="C.36.3" sheetId="26" r:id="rId26"/>
-    <sheet name="PDI85.1" sheetId="30" r:id="rId27"/>
-    <sheet name="PDI85.2" sheetId="31" r:id="rId28"/>
-    <sheet name="PDI86" sheetId="29" r:id="rId29"/>
-    <sheet name="PDI91" sheetId="28" r:id="rId30"/>
-    <sheet name="PDI93" sheetId="27" r:id="rId31"/>
-    <sheet name="B.1.623" sheetId="32" r:id="rId32"/>
-    <sheet name="B.1.621" sheetId="33" r:id="rId33"/>
-    <sheet name="P.4" sheetId="34" r:id="rId34"/>
-    <sheet name="A.29" sheetId="35" r:id="rId35"/>
+    <sheet name="C.36.3.1" sheetId="37" r:id="rId27"/>
+    <sheet name="PDI85.1" sheetId="30" r:id="rId28"/>
+    <sheet name="PDI85.2" sheetId="31" r:id="rId29"/>
+    <sheet name="PDI86" sheetId="29" r:id="rId30"/>
+    <sheet name="PDI91" sheetId="28" r:id="rId31"/>
+    <sheet name="PDI93" sheetId="27" r:id="rId32"/>
+    <sheet name="B.1.623" sheetId="32" r:id="rId33"/>
+    <sheet name="B.1.621" sheetId="33" r:id="rId34"/>
+    <sheet name="P.4" sheetId="34" r:id="rId35"/>
+    <sheet name="A.29" sheetId="35" r:id="rId36"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7399" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7645" uniqueCount="1023">
   <si>
     <t>Position</t>
   </si>
@@ -3082,6 +3083,51 @@
   </si>
   <si>
     <t>3'UTR:29739</t>
+  </si>
+  <si>
+    <t>N1329N</t>
+  </si>
+  <si>
+    <t>NSP3:N1329N</t>
+  </si>
+  <si>
+    <t>P529L</t>
+  </si>
+  <si>
+    <t>NSP13:P529L</t>
+  </si>
+  <si>
+    <t>T50T</t>
+  </si>
+  <si>
+    <t>NSP14:T50T</t>
+  </si>
+  <si>
+    <t>A845S</t>
+  </si>
+  <si>
+    <t>S:A845S</t>
+  </si>
+  <si>
+    <t>Y113H</t>
+  </si>
+  <si>
+    <t>ORF3a:Y113H</t>
+  </si>
+  <si>
+    <t>K256R</t>
+  </si>
+  <si>
+    <t>N:K256R</t>
+  </si>
+  <si>
+    <t>N25N</t>
+  </si>
+  <si>
+    <t>ORF10:N25N</t>
+  </si>
+  <si>
+    <t>deletion_extragenic</t>
   </si>
 </sst>
 </file>
@@ -10887,7 +10933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -20199,10 +20245,1045 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>569</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E2" t="s">
+        <v>741</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>345</v>
+      </c>
+      <c r="H2" t="s">
+        <v>742</v>
+      </c>
+      <c r="I2">
+        <v>98.445595854922274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2841</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>743</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" t="s">
+        <v>744</v>
+      </c>
+      <c r="I3">
+        <v>94.818652849740943</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5180</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>745</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>746</v>
+      </c>
+      <c r="I4">
+        <v>99.481865284974091</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6706</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="I5">
+        <v>99.481865284974091</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7124</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>568</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
+        <v>569</v>
+      </c>
+      <c r="I6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>9203</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" t="s">
+        <v>717</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" t="s">
+        <v>718</v>
+      </c>
+      <c r="I7">
+        <v>99.481865284974091</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9929</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" t="s">
+        <v>747</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" t="s">
+        <v>748</v>
+      </c>
+      <c r="I8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>11325</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" t="s">
+        <v>749</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" t="s">
+        <v>750</v>
+      </c>
+      <c r="I9">
+        <v>98.963730569948183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>11337</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" t="s">
+        <v>751</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s">
+        <v>752</v>
+      </c>
+      <c r="I10">
+        <v>99.481865284974091</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>16549</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" t="s">
+        <v>753</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>179</v>
+      </c>
+      <c r="H11" t="s">
+        <v>754</v>
+      </c>
+      <c r="I11">
+        <v>98.963730569948183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>17766</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E12" t="s">
+        <v>755</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
+        <v>179</v>
+      </c>
+      <c r="H12" t="s">
+        <v>756</v>
+      </c>
+      <c r="I12">
+        <v>99.481865284974091</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>17822</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>177</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>179</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1011</v>
+      </c>
+      <c r="I13">
+        <v>99.481865284974091</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>18189</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>120</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1013</v>
+      </c>
+      <c r="I14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>21597</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>757</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>758</v>
+      </c>
+      <c r="I15">
+        <v>99.481865284974091</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>21765</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>736</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>380</v>
+      </c>
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>381</v>
+      </c>
+      <c r="I16">
+        <v>74.093264248704656</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>21766</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>736</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>380</v>
+      </c>
+      <c r="F17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" t="s">
+        <v>381</v>
+      </c>
+      <c r="I17">
+        <v>74.093264248704656</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>21767</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>736</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>380</v>
+      </c>
+      <c r="F18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" t="s">
+        <v>381</v>
+      </c>
+      <c r="I18">
+        <v>74.093264248704656</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>21768</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>736</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>380</v>
+      </c>
+      <c r="F19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" t="s">
+        <v>381</v>
+      </c>
+      <c r="I19">
+        <v>74.093264248704656</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>21769</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>736</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>380</v>
+      </c>
+      <c r="F20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" t="s">
+        <v>381</v>
+      </c>
+      <c r="I20">
+        <v>74.093264248704656</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21770</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>736</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>380</v>
+      </c>
+      <c r="F21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" t="s">
+        <v>381</v>
+      </c>
+      <c r="I21">
+        <v>74.093264248704656</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22016</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>759</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" t="s">
+        <v>760</v>
+      </c>
+      <c r="I22">
+        <v>97.92746113989638</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22600</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>761</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" t="s">
+        <v>762</v>
+      </c>
+      <c r="I23">
+        <v>99.481865284974091</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22917</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" t="s">
+        <v>90</v>
+      </c>
+      <c r="I24">
+        <v>99.481865284974091</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22992</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>386</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" t="s">
+        <v>387</v>
+      </c>
+      <c r="I25">
+        <v>98.963730569948183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23593</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>295</v>
+      </c>
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" t="s">
+        <v>296</v>
+      </c>
+      <c r="I26">
+        <v>99.481865284974091</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>24095</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1014</v>
+      </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" t="s">
+        <v>1015</v>
+      </c>
+      <c r="I27">
+        <v>84.974093264248708</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>24257</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>763</v>
+      </c>
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" t="s">
+        <v>764</v>
+      </c>
+      <c r="I28">
+        <v>92.746113989637308</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>24811</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>804</v>
+      </c>
+      <c r="F29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" t="s">
+        <v>805</v>
+      </c>
+      <c r="I29">
+        <v>99.481865284974091</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>25729</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1016</v>
+      </c>
+      <c r="F30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" t="s">
+        <v>46</v>
+      </c>
+      <c r="H30" t="s">
+        <v>1017</v>
+      </c>
+      <c r="I30">
+        <v>98.963730569948183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>26767</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" t="s">
+        <v>303</v>
+      </c>
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" t="s">
+        <v>106</v>
+      </c>
+      <c r="H31" t="s">
+        <v>304</v>
+      </c>
+      <c r="I31">
+        <v>98.445595854922274</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>27882</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>399</v>
+      </c>
+      <c r="E32" t="s">
+        <v>765</v>
+      </c>
+      <c r="F32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" t="s">
+        <v>401</v>
+      </c>
+      <c r="H32" t="s">
+        <v>766</v>
+      </c>
+      <c r="I32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>28273</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>736</v>
+      </c>
+      <c r="D33" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33">
+        <v>28273</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1022</v>
+      </c>
+      <c r="G33" t="s">
+        <v>50</v>
+      </c>
+      <c r="H33" t="s">
+        <v>99</v>
+      </c>
+      <c r="I33">
+        <v>97.409326424870471</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>29040</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" t="s">
+        <v>1019</v>
+      </c>
+      <c r="I34">
+        <v>98.963730569948183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>29632</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F35" t="s">
+        <v>21</v>
+      </c>
+      <c r="G35" t="s">
+        <v>146</v>
+      </c>
+      <c r="H35" t="s">
+        <v>1021</v>
+      </c>
+      <c r="I35">
+        <v>99.481865284974091</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21201,7 +22282,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
@@ -21899,833 +22980,6 @@
         <v>92.452830188679243</v>
       </c>
       <c r="J23" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5175</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>818</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" t="s">
-        <v>819</v>
-      </c>
-      <c r="I2" s="1">
-        <v>93.333333333333329</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>8950</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>820</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" t="s">
-        <v>821</v>
-      </c>
-      <c r="I3" s="1">
-        <v>93.333333333333329</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>9891</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" s="1">
-        <v>93.333333333333329</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>10264</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>140</v>
-      </c>
-      <c r="E5" t="s">
-        <v>822</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>142</v>
-      </c>
-      <c r="H5" t="s">
-        <v>823</v>
-      </c>
-      <c r="I5" s="1">
-        <v>93.333333333333329</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>11152</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" t="s">
-        <v>824</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" t="s">
-        <v>825</v>
-      </c>
-      <c r="I6" s="1">
-        <v>93.333333333333329</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>11450</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" t="s">
-        <v>826</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" t="s">
-        <v>827</v>
-      </c>
-      <c r="I7" s="1">
-        <v>93.333333333333329</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>13275</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>795</v>
-      </c>
-      <c r="E8" t="s">
-        <v>828</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" t="s">
-        <v>829</v>
-      </c>
-      <c r="H8" t="s">
-        <v>830</v>
-      </c>
-      <c r="I8" s="1">
-        <v>93.333333333333329</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>14103</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" t="s">
-        <v>831</v>
-      </c>
-      <c r="F9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" t="s">
-        <v>832</v>
-      </c>
-      <c r="I9" s="1">
-        <v>93.333333333333329</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>14571</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" t="s">
-        <v>833</v>
-      </c>
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" t="s">
-        <v>834</v>
-      </c>
-      <c r="I10" s="1">
-        <v>93.333333333333329</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>21568</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" t="s">
-        <v>836</v>
-      </c>
-      <c r="I11" s="1">
-        <v>93.333333333333329</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>21602</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>837</v>
-      </c>
-      <c r="F12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" t="s">
-        <v>838</v>
-      </c>
-      <c r="I12" s="1">
-        <v>93.333333333333329</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>21721</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>839</v>
-      </c>
-      <c r="F13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" t="s">
-        <v>840</v>
-      </c>
-      <c r="I13" s="1">
-        <v>93.333333333333329</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>21846</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
-        <v>327</v>
-      </c>
-      <c r="F14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" t="s">
-        <v>328</v>
-      </c>
-      <c r="I14" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>21986</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>736</v>
-      </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" t="s">
-        <v>841</v>
-      </c>
-      <c r="F15" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" t="s">
-        <v>842</v>
-      </c>
-      <c r="I15" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>21987</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>736</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" t="s">
-        <v>841</v>
-      </c>
-      <c r="F16" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" t="s">
-        <v>842</v>
-      </c>
-      <c r="I16" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>21988</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>736</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" t="s">
-        <v>841</v>
-      </c>
-      <c r="F17" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" t="s">
-        <v>842</v>
-      </c>
-      <c r="I17" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>21989</v>
-      </c>
-      <c r="B18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>736</v>
-      </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" t="s">
-        <v>841</v>
-      </c>
-      <c r="F18" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" t="s">
-        <v>842</v>
-      </c>
-      <c r="I18" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>21990</v>
-      </c>
-      <c r="B19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" t="s">
-        <v>736</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" t="s">
-        <v>841</v>
-      </c>
-      <c r="F19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" t="s">
-        <v>842</v>
-      </c>
-      <c r="I19" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>21991</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" t="s">
-        <v>736</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" t="s">
-        <v>841</v>
-      </c>
-      <c r="F20" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" t="s">
-        <v>842</v>
-      </c>
-      <c r="I20" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>21993</v>
-      </c>
-      <c r="B21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s">
-        <v>740</v>
-      </c>
-      <c r="D21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" t="s">
-        <v>843</v>
-      </c>
-      <c r="F21" t="s">
-        <v>150</v>
-      </c>
-      <c r="G21" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" t="s">
-        <v>844</v>
-      </c>
-      <c r="I21" s="1">
-        <v>73.333333333333329</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>23012</v>
-      </c>
-      <c r="B22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" t="s">
-        <v>504</v>
-      </c>
-      <c r="F22" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" t="s">
-        <v>505</v>
-      </c>
-      <c r="I22" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>23064</v>
-      </c>
-      <c r="B23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" t="s">
-        <v>845</v>
-      </c>
-      <c r="F23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" t="s">
-        <v>846</v>
-      </c>
-      <c r="I23" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>24904</v>
-      </c>
-      <c r="B24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" t="s">
-        <v>847</v>
-      </c>
-      <c r="F24" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" t="s">
-        <v>848</v>
-      </c>
-      <c r="I24" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>25906</v>
-      </c>
-      <c r="B25" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" t="s">
-        <v>816</v>
-      </c>
-      <c r="F25" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" t="s">
-        <v>46</v>
-      </c>
-      <c r="H25" t="s">
-        <v>817</v>
-      </c>
-      <c r="I25" s="1">
-        <v>73.333333333333329</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>28271</v>
-      </c>
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26">
-        <v>28271</v>
-      </c>
-      <c r="F26" t="s">
-        <v>49</v>
-      </c>
-      <c r="G26" t="s">
-        <v>50</v>
-      </c>
-      <c r="H26" t="s">
-        <v>394</v>
-      </c>
-      <c r="I26" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>28531</v>
-      </c>
-      <c r="B27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" t="s">
-        <v>849</v>
-      </c>
-      <c r="F27" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" t="s">
-        <v>22</v>
-      </c>
-      <c r="H27" t="s">
-        <v>850</v>
-      </c>
-      <c r="I27" s="1">
-        <v>93.333333333333329</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>28917</v>
-      </c>
-      <c r="B28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" t="s">
-        <v>851</v>
-      </c>
-      <c r="F28" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" t="s">
-        <v>852</v>
-      </c>
-      <c r="I28" s="1">
-        <v>93.333333333333329</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23516,6 +23770,833 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5175</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>818</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" t="s">
+        <v>819</v>
+      </c>
+      <c r="I2" s="1">
+        <v>93.333333333333329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>8950</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>820</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" t="s">
+        <v>821</v>
+      </c>
+      <c r="I3" s="1">
+        <v>93.333333333333329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>9891</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="1">
+        <v>93.333333333333329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10264</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" t="s">
+        <v>822</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H5" t="s">
+        <v>823</v>
+      </c>
+      <c r="I5" s="1">
+        <v>93.333333333333329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>11152</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" t="s">
+        <v>824</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" t="s">
+        <v>825</v>
+      </c>
+      <c r="I6" s="1">
+        <v>93.333333333333329</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11450</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" t="s">
+        <v>826</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" t="s">
+        <v>827</v>
+      </c>
+      <c r="I7" s="1">
+        <v>93.333333333333329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>13275</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>795</v>
+      </c>
+      <c r="E8" t="s">
+        <v>828</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>829</v>
+      </c>
+      <c r="H8" t="s">
+        <v>830</v>
+      </c>
+      <c r="I8" s="1">
+        <v>93.333333333333329</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>14103</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>831</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>832</v>
+      </c>
+      <c r="I9" s="1">
+        <v>93.333333333333329</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>14571</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>833</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" t="s">
+        <v>834</v>
+      </c>
+      <c r="I10" s="1">
+        <v>93.333333333333329</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>21568</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>835</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" t="s">
+        <v>836</v>
+      </c>
+      <c r="I11" s="1">
+        <v>93.333333333333329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>21602</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>837</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" t="s">
+        <v>838</v>
+      </c>
+      <c r="I12" s="1">
+        <v>93.333333333333329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>21721</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>839</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>840</v>
+      </c>
+      <c r="I13" s="1">
+        <v>93.333333333333329</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>21846</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>327</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>328</v>
+      </c>
+      <c r="I14" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>21986</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>736</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>841</v>
+      </c>
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>842</v>
+      </c>
+      <c r="I15" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>21987</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>736</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>841</v>
+      </c>
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>842</v>
+      </c>
+      <c r="I16" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>21988</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>736</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>841</v>
+      </c>
+      <c r="F17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" t="s">
+        <v>842</v>
+      </c>
+      <c r="I17" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>21989</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>736</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>841</v>
+      </c>
+      <c r="F18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" t="s">
+        <v>842</v>
+      </c>
+      <c r="I18" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>21990</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>736</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>841</v>
+      </c>
+      <c r="F19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" t="s">
+        <v>842</v>
+      </c>
+      <c r="I19" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>21991</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>736</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>841</v>
+      </c>
+      <c r="F20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" t="s">
+        <v>842</v>
+      </c>
+      <c r="I20" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21993</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>740</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>843</v>
+      </c>
+      <c r="F21" t="s">
+        <v>150</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" t="s">
+        <v>844</v>
+      </c>
+      <c r="I21" s="1">
+        <v>73.333333333333329</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>23012</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>504</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" t="s">
+        <v>505</v>
+      </c>
+      <c r="I22" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23064</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>845</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" t="s">
+        <v>846</v>
+      </c>
+      <c r="I23" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24904</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>847</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" t="s">
+        <v>848</v>
+      </c>
+      <c r="I24" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25906</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>816</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" t="s">
+        <v>46</v>
+      </c>
+      <c r="H25" t="s">
+        <v>817</v>
+      </c>
+      <c r="I25" s="1">
+        <v>73.333333333333329</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>28271</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26">
+        <v>28271</v>
+      </c>
+      <c r="F26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" t="s">
+        <v>394</v>
+      </c>
+      <c r="I26" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>28531</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" t="s">
+        <v>849</v>
+      </c>
+      <c r="F27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" t="s">
+        <v>850</v>
+      </c>
+      <c r="I27" s="1">
+        <v>93.333333333333329</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28917</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" t="s">
+        <v>851</v>
+      </c>
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" t="s">
+        <v>852</v>
+      </c>
+      <c r="I28" s="1">
+        <v>93.333333333333329</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23935,7 +25016,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
@@ -25287,7 +26368,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I53"/>
   <sheetViews>
@@ -26843,7 +27924,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
@@ -27815,7 +28896,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
@@ -28471,7 +29552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>

</xml_diff>

<commit_message>
if QC fail - write in Variant column
</commit_message>
<xml_diff>
--- a/mutationsTable.xlsx
+++ b/mutationsTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" tabRatio="846" firstSheet="15" activeTab="26"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" tabRatio="846" firstSheet="16" activeTab="35"/>
   </bookViews>
   <sheets>
     <sheet name="B.1.1.7" sheetId="13" r:id="rId1"/>
@@ -3499,7 +3499,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3555,7 +3555,7 @@
         <v>28273</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>45</v>
+        <v>1022</v>
       </c>
       <c r="G2" t="s">
         <v>50</v>
@@ -4707,8 +4707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6046,7 +6046,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7126,8 +7126,8 @@
       <c r="E37">
         <v>27387</v>
       </c>
-      <c r="F37" t="s">
-        <v>45</v>
+      <c r="F37" s="6" t="s">
+        <v>1022</v>
       </c>
       <c r="G37" t="s">
         <v>50</v>
@@ -10854,7 +10854,7 @@
         <v>28273</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>45</v>
+        <v>1022</v>
       </c>
       <c r="G22" t="s">
         <v>50</v>
@@ -10934,7 +10934,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11684,8 +11684,8 @@
       <c r="E26">
         <v>28273</v>
       </c>
-      <c r="F26" t="s">
-        <v>45</v>
+      <c r="F26" s="6" t="s">
+        <v>1022</v>
       </c>
       <c r="G26" t="s">
         <v>50</v>
@@ -12507,7 +12507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
@@ -13918,7 +13918,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:C28"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15194,8 +15194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16440,7 +16440,7 @@
         <v>52</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>45</v>
+        <v>1022</v>
       </c>
       <c r="G43" t="s">
         <v>50</v>
@@ -16469,7 +16469,7 @@
         <v>52</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>45</v>
+        <v>1022</v>
       </c>
       <c r="G44" t="s">
         <v>50</v>
@@ -16971,7 +16971,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19475,7 +19475,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20225,8 +20225,8 @@
       <c r="E26">
         <v>28273</v>
       </c>
-      <c r="F26" t="s">
-        <v>45</v>
+      <c r="F26" s="6" t="s">
+        <v>1022</v>
       </c>
       <c r="G26" t="s">
         <v>50</v>
@@ -20247,7 +20247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
@@ -21283,7 +21283,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22235,8 +22235,8 @@
       <c r="E33">
         <v>28273</v>
       </c>
-      <c r="F33" t="s">
-        <v>45</v>
+      <c r="F33" s="6" t="s">
+        <v>1022</v>
       </c>
       <c r="G33" t="s">
         <v>50</v>
@@ -22991,7 +22991,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23047,7 +23047,7 @@
         <v>28273</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>45</v>
+        <v>1022</v>
       </c>
       <c r="G2" t="s">
         <v>50</v>
@@ -25020,7 +25020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
@@ -27929,7 +27929,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29556,8 +29556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30364,8 +30364,8 @@
       <c r="E28">
         <v>28273</v>
       </c>
-      <c r="F28" t="s">
-        <v>45</v>
+      <c r="F28" s="6" t="s">
+        <v>1022</v>
       </c>
       <c r="G28" t="s">
         <v>50</v>
@@ -30503,7 +30503,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31379,7 +31379,7 @@
         <v>28273</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>45</v>
+        <v>1022</v>
       </c>
       <c r="G30" t="s">
         <v>50</v>
@@ -31400,7 +31400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -33332,7 +33332,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:H13"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33872,7 +33872,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F29" sqref="E29:F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34921,7 +34921,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
variants names as written in variants catalog (icvl)
</commit_message>
<xml_diff>
--- a/mutationsTable.xlsx
+++ b/mutationsTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" tabRatio="846" firstSheet="16" activeTab="35"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" tabRatio="846" firstSheet="6" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="B.1.1.7" sheetId="13" r:id="rId1"/>
@@ -35,8 +35,8 @@
     <sheet name="P.1" sheetId="21" r:id="rId21"/>
     <sheet name="P.3" sheetId="22" r:id="rId22"/>
     <sheet name="P.2" sheetId="23" r:id="rId23"/>
-    <sheet name="VUI_P681H_Israel" sheetId="24" r:id="rId24"/>
-    <sheet name="VUI_L452R|L1063F_Israel" sheetId="25" r:id="rId25"/>
+    <sheet name="ISR_B.1.1.50+P681H" sheetId="24" r:id="rId24"/>
+    <sheet name="ISR_B.1.362+L452R" sheetId="25" r:id="rId25"/>
     <sheet name="C.36.3" sheetId="26" r:id="rId26"/>
     <sheet name="C.36.3.1" sheetId="37" r:id="rId27"/>
     <sheet name="PDI85.1" sheetId="30" r:id="rId28"/>
@@ -3499,7 +3499,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19372,7 +19372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="V42" sqref="V42"/>
     </sheetView>
   </sheetViews>
@@ -29556,7 +29556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed empty rows in mutationsTable.xlsx
</commit_message>
<xml_diff>
--- a/mutationsTable.xlsx
+++ b/mutationsTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" tabRatio="846" firstSheet="15" activeTab="27"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" tabRatio="846" firstSheet="4" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="B.1.1.7" sheetId="13" r:id="rId1"/>
@@ -5967,7 +5967,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O44" sqref="O44"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6586,7 +6586,6 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>A21+1</f>
         <v>28249</v>
       </c>
       <c r="B22" t="s">
@@ -6616,7 +6615,6 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" ref="A23:A26" si="0">A22+1</f>
         <v>28250</v>
       </c>
       <c r="B23" t="s">
@@ -6646,7 +6644,6 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="0"/>
         <v>28251</v>
       </c>
       <c r="B24" t="s">
@@ -6676,7 +6673,6 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="0"/>
         <v>28252</v>
       </c>
       <c r="B25" t="s">
@@ -6706,7 +6702,6 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="0"/>
         <v>28253</v>
       </c>
       <c r="B26" t="s">
@@ -6823,7 +6818,6 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>A29+1</f>
         <v>26164</v>
       </c>
       <c r="B30" t="s">
@@ -6852,9 +6846,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="e">
-        <f>#REF!+1</f>
-        <v>#REF!</v>
+      <c r="A31">
+        <v>26164</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -6882,9 +6875,8 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="e">
-        <f t="shared" ref="A32:A35" si="1">A31+1</f>
-        <v>#REF!</v>
+      <c r="A32">
+        <v>26165</v>
       </c>
       <c r="B32" t="s">
         <v>30</v>
@@ -6912,9 +6904,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="A33">
+        <v>26165</v>
       </c>
       <c r="B33" t="s">
         <v>16</v>
@@ -6942,9 +6933,8 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="A34">
+        <v>26166</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -6972,9 +6962,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="A35">
+        <v>26166</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -8414,7 +8403,7 @@
   <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O44" sqref="O44"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9062,7 +9051,6 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>A22+1</f>
         <v>21969</v>
       </c>
       <c r="B23" t="s">
@@ -9092,7 +9080,6 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" ref="A24:A47" si="0">A23+1</f>
         <v>21970</v>
       </c>
       <c r="B24" t="s">
@@ -9122,7 +9109,6 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="0"/>
         <v>21971</v>
       </c>
       <c r="B25" t="s">
@@ -9152,7 +9138,6 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="0"/>
         <v>21972</v>
       </c>
       <c r="B26" t="s">
@@ -9182,7 +9167,6 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="0"/>
         <v>21973</v>
       </c>
       <c r="B27" t="s">
@@ -9212,7 +9196,6 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="0"/>
         <v>21974</v>
       </c>
       <c r="B28" t="s">
@@ -9242,7 +9225,6 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="0"/>
         <v>21975</v>
       </c>
       <c r="B29" t="s">
@@ -9272,7 +9254,6 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="0"/>
         <v>21976</v>
       </c>
       <c r="B30" t="s">
@@ -9301,9 +9282,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="e">
-        <f>#REF!+1</f>
-        <v>#REF!</v>
+      <c r="A31">
+        <v>21977</v>
       </c>
       <c r="B31" t="s">
         <v>9</v>
@@ -9331,9 +9311,8 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A32">
+        <v>21978</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -9361,9 +9340,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A33">
+        <v>21979</v>
       </c>
       <c r="B33" t="s">
         <v>16</v>
@@ -9391,9 +9369,8 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A34">
+        <v>21980</v>
       </c>
       <c r="B34" t="s">
         <v>16</v>
@@ -9421,9 +9398,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A35">
+        <v>21981</v>
       </c>
       <c r="B35" t="s">
         <v>16</v>
@@ -9451,9 +9427,8 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A36">
+        <v>21982</v>
       </c>
       <c r="B36" t="s">
         <v>16</v>
@@ -9481,9 +9456,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A37">
+        <v>21983</v>
       </c>
       <c r="B37" t="s">
         <v>16</v>
@@ -9511,9 +9485,8 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A38">
+        <v>21984</v>
       </c>
       <c r="B38" t="s">
         <v>30</v>
@@ -9541,9 +9514,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A39">
+        <v>21985</v>
       </c>
       <c r="B39" t="s">
         <v>30</v>
@@ -9571,9 +9543,8 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A40">
+        <v>21986</v>
       </c>
       <c r="B40" t="s">
         <v>30</v>
@@ -9601,9 +9572,8 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A41">
+        <v>21987</v>
       </c>
       <c r="B41" t="s">
         <v>16</v>
@@ -9631,9 +9601,8 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A42">
+        <v>21988</v>
       </c>
       <c r="B42" t="s">
         <v>30</v>
@@ -9661,9 +9630,8 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A43">
+        <v>21989</v>
       </c>
       <c r="B43" t="s">
         <v>16</v>
@@ -9691,9 +9659,8 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A44">
+        <v>21990</v>
       </c>
       <c r="B44" t="s">
         <v>16</v>
@@ -9721,9 +9688,8 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A45">
+        <v>21991</v>
       </c>
       <c r="B45" t="s">
         <v>16</v>
@@ -9751,9 +9717,8 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A46">
+        <v>21992</v>
       </c>
       <c r="B46" t="s">
         <v>10</v>
@@ -9781,9 +9746,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A47">
+        <v>21993</v>
       </c>
       <c r="B47" t="s">
         <v>16</v>
@@ -12336,8 +12300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O44" sqref="O44"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12435,7 +12399,6 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>A3+1</f>
         <v>11289</v>
       </c>
       <c r="B4" t="s">
@@ -12465,7 +12428,6 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" ref="A5:A11" si="0">A4+1</f>
         <v>11290</v>
       </c>
       <c r="B5" t="s">
@@ -12495,7 +12457,6 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="0"/>
         <v>11291</v>
       </c>
       <c r="B6" t="s">
@@ -12525,7 +12486,6 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="0"/>
         <v>11292</v>
       </c>
       <c r="B7" t="s">
@@ -12555,7 +12515,6 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="0"/>
         <v>11293</v>
       </c>
       <c r="B8" t="s">
@@ -12585,7 +12544,6 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="0"/>
         <v>11294</v>
       </c>
       <c r="B9" t="s">
@@ -12615,7 +12573,6 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="0"/>
         <v>11295</v>
       </c>
       <c r="B10" t="s">
@@ -12645,7 +12602,6 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="0"/>
         <v>11296</v>
       </c>
       <c r="B11" t="s">
@@ -13081,7 +13037,6 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>A25+1</f>
         <v>22300</v>
       </c>
       <c r="B26" t="s">
@@ -13111,7 +13066,6 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" ref="A27:A44" si="1">A26+1</f>
         <v>22301</v>
       </c>
       <c r="B27" t="s">
@@ -13141,7 +13095,6 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="1"/>
         <v>22302</v>
       </c>
       <c r="B28" t="s">
@@ -13171,7 +13124,6 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="1"/>
         <v>22303</v>
       </c>
       <c r="B29" t="s">
@@ -13201,7 +13153,6 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="1"/>
         <v>22304</v>
       </c>
       <c r="B30" t="s">
@@ -13230,9 +13181,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="e">
-        <f>#REF!+1</f>
-        <v>#REF!</v>
+      <c r="A31">
+        <v>22305</v>
       </c>
       <c r="B31" t="s">
         <v>16</v>
@@ -13260,9 +13210,8 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="A32">
+        <v>22306</v>
       </c>
       <c r="B32" t="s">
         <v>16</v>
@@ -13290,9 +13239,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="A33">
+        <v>22307</v>
       </c>
       <c r="B33" t="s">
         <v>16</v>
@@ -13320,9 +13268,8 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="A34">
+        <v>22308</v>
       </c>
       <c r="B34" t="s">
         <v>30</v>
@@ -13350,9 +13297,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="A35">
+        <v>22309</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -13380,9 +13326,8 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="A36">
+        <v>22310</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
@@ -13410,9 +13355,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="A37">
+        <v>22311</v>
       </c>
       <c r="B37" t="s">
         <v>16</v>
@@ -13440,9 +13384,8 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="A38">
+        <v>22312</v>
       </c>
       <c r="B38" t="s">
         <v>9</v>
@@ -13470,9 +13413,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="A39">
+        <v>22313</v>
       </c>
       <c r="B39" t="s">
         <v>9</v>
@@ -13500,9 +13442,8 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="A40">
+        <v>22314</v>
       </c>
       <c r="B40" t="s">
         <v>16</v>
@@ -13530,9 +13471,8 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="A41">
+        <v>22315</v>
       </c>
       <c r="B41" t="s">
         <v>30</v>
@@ -13560,9 +13500,8 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="A42">
+        <v>22316</v>
       </c>
       <c r="B42" t="s">
         <v>30</v>
@@ -13590,9 +13529,8 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="A43">
+        <v>22317</v>
       </c>
       <c r="B43" t="s">
         <v>16</v>
@@ -13620,9 +13558,8 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="A44">
+        <v>22318</v>
       </c>
       <c r="B44" t="s">
         <v>30</v>
@@ -13651,7 +13588,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>24138</v>
+        <v>22319</v>
       </c>
       <c r="B45" t="s">
         <v>9</v>
@@ -13716,7 +13653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
@@ -20994,7 +20931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
@@ -30968,7 +30905,7 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O44" sqref="O44"/>
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31616,7 +31553,6 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>A22+1</f>
         <v>27268</v>
       </c>
       <c r="B23" t="s">
@@ -31646,7 +31582,6 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" ref="A24:A49" si="0">A23+1</f>
         <v>27269</v>
       </c>
       <c r="B24" t="s">
@@ -31676,7 +31611,6 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="0"/>
         <v>27270</v>
       </c>
       <c r="B25" t="s">
@@ -31706,7 +31640,6 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="0"/>
         <v>27271</v>
       </c>
       <c r="B26" t="s">
@@ -31736,7 +31669,6 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="0"/>
         <v>27272</v>
       </c>
       <c r="B27" t="s">
@@ -31766,7 +31698,6 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="0"/>
         <v>27273</v>
       </c>
       <c r="B28" t="s">
@@ -31796,7 +31727,6 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="0"/>
         <v>27274</v>
       </c>
       <c r="B29" t="s">
@@ -31826,7 +31756,6 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="0"/>
         <v>27275</v>
       </c>
       <c r="B30" t="s">
@@ -31855,9 +31784,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="e">
-        <f>#REF!+1</f>
-        <v>#REF!</v>
+      <c r="A31">
+        <v>27276</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -31885,9 +31813,8 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A32">
+        <v>27277</v>
       </c>
       <c r="B32" t="s">
         <v>16</v>
@@ -31915,9 +31842,8 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A33">
+        <v>27278</v>
       </c>
       <c r="B33" t="s">
         <v>16</v>
@@ -31945,9 +31871,8 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A34">
+        <v>27279</v>
       </c>
       <c r="B34" t="s">
         <v>16</v>
@@ -31975,9 +31900,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A35">
+        <v>27280</v>
       </c>
       <c r="B35" t="s">
         <v>30</v>
@@ -32005,9 +31929,8 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A36">
+        <v>27281</v>
       </c>
       <c r="B36" t="s">
         <v>30</v>
@@ -32035,9 +31958,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A37">
+        <v>27282</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
@@ -32065,9 +31987,8 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A38">
+        <v>27283</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
@@ -32095,9 +32016,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A39">
+        <v>27284</v>
       </c>
       <c r="B39" t="s">
         <v>16</v>
@@ -32125,9 +32045,8 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A40">
+        <v>27285</v>
       </c>
       <c r="B40" t="s">
         <v>9</v>
@@ -32155,9 +32074,8 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A41">
+        <v>27286</v>
       </c>
       <c r="B41" t="s">
         <v>16</v>
@@ -32185,9 +32103,8 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A42">
+        <v>27287</v>
       </c>
       <c r="B42" t="s">
         <v>16</v>
@@ -32215,9 +32132,8 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A43">
+        <v>27288</v>
       </c>
       <c r="B43" t="s">
         <v>30</v>
@@ -32245,9 +32161,8 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A44">
+        <v>27289</v>
       </c>
       <c r="B44" t="s">
         <v>10</v>
@@ -32275,9 +32190,8 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A45">
+        <v>27290</v>
       </c>
       <c r="B45" t="s">
         <v>16</v>
@@ -32305,9 +32219,8 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A46">
+        <v>27291</v>
       </c>
       <c r="B46" t="s">
         <v>16</v>
@@ -32335,9 +32248,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A47">
+        <v>27292</v>
       </c>
       <c r="B47" t="s">
         <v>10</v>
@@ -32365,9 +32277,8 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A48">
+        <v>27293</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
@@ -32395,9 +32306,8 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
+      <c r="A49">
+        <v>27294</v>
       </c>
       <c r="B49" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
added new variant AW.1
</commit_message>
<xml_diff>
--- a/mutationsTable.xlsx
+++ b/mutationsTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" tabRatio="846" firstSheet="9" activeTab="26"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" tabRatio="846" firstSheet="16" activeTab="36"/>
   </bookViews>
   <sheets>
     <sheet name="B.1.1.7" sheetId="13" r:id="rId1"/>
@@ -48,6 +48,7 @@
     <sheet name="B.1.621" sheetId="33" r:id="rId34"/>
     <sheet name="P.4" sheetId="34" r:id="rId35"/>
     <sheet name="A.29" sheetId="35" r:id="rId36"/>
+    <sheet name="AW.1" sheetId="38" r:id="rId37"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7487" uniqueCount="1010">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7580" uniqueCount="1030">
   <si>
     <t>Position</t>
   </si>
@@ -3089,6 +3090,66 @@
   </si>
   <si>
     <t>extragenic_deletion</t>
+  </si>
+  <si>
+    <t>T634I</t>
+  </si>
+  <si>
+    <t>NSP2:T634I</t>
+  </si>
+  <si>
+    <t>T350N</t>
+  </si>
+  <si>
+    <t>NSP3:T350N</t>
+  </si>
+  <si>
+    <t>H389H</t>
+  </si>
+  <si>
+    <t>NSP4:H389H</t>
+  </si>
+  <si>
+    <t>T141T</t>
+  </si>
+  <si>
+    <t>NSP8:T141T</t>
+  </si>
+  <si>
+    <t>T21T</t>
+  </si>
+  <si>
+    <t>NSP9:T21T</t>
+  </si>
+  <si>
+    <t>T111I</t>
+  </si>
+  <si>
+    <t>NSP10:T111I</t>
+  </si>
+  <si>
+    <t>E365D</t>
+  </si>
+  <si>
+    <t>NSP13:E365D</t>
+  </si>
+  <si>
+    <t>D375D</t>
+  </si>
+  <si>
+    <t>NSP14:D375D</t>
+  </si>
+  <si>
+    <t>T112I</t>
+  </si>
+  <si>
+    <t>NSP15:T112I</t>
+  </si>
+  <si>
+    <t>A188S</t>
+  </si>
+  <si>
+    <t>NSP16:A188S</t>
   </si>
 </sst>
 </file>
@@ -3157,7 +3218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3175,6 +3236,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -19027,7 +19089,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O44" sqref="O44"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19797,10 +19859,10 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z11" sqref="Z11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20420,379 +20482,408 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="11">
         <v>22016</v>
       </c>
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="11" t="s">
         <v>750</v>
       </c>
-      <c r="F22" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="F22" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="11" t="s">
         <v>751</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="11">
         <v>97.92746113989638</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="11">
         <v>22600</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C23" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="11" t="s">
         <v>752</v>
       </c>
-      <c r="F23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="F23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="11" t="s">
         <v>753</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="11">
         <v>99.481865284974091</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="11">
         <v>22917</v>
       </c>
-      <c r="B24" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="F24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="F24" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="11">
         <v>99.481865284974091</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="11">
         <v>22992</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="11" t="s">
         <v>386</v>
       </c>
-      <c r="F25" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="F25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="11">
         <v>98.963730569948183</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="11">
         <v>23593</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C26" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="F26" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="F26" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="11">
         <v>99.481865284974091</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="11">
         <v>24095</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="C27" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="11" t="s">
         <v>1000</v>
       </c>
-      <c r="F27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="F27" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="11" t="s">
         <v>1001</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="11">
         <v>84.974093264248708</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="11">
         <v>24257</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C28" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C28" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="11" t="s">
         <v>754</v>
       </c>
-      <c r="F28" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="F28" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="11" t="s">
         <v>755</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="11">
         <v>92.746113989637308</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="11">
         <v>24811</v>
       </c>
-      <c r="B29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="B29" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="11" t="s">
         <v>795</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="11" t="s">
         <v>796</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="11">
         <v>99.481865284974091</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="11">
         <v>25729</v>
       </c>
-      <c r="B30" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="B30" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="11" t="s">
         <v>1002</v>
       </c>
-      <c r="F30" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="F30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="11" t="s">
         <v>1003</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="11">
         <v>98.963730569948183</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="11">
+        <v>26767</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="I31" s="11">
+        <v>98.445595854922274</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
         <v>27882</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C31" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C32" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" s="11" t="s">
         <v>756</v>
       </c>
-      <c r="F31" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="F32" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="11" t="s">
         <v>401</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H32" s="11" t="s">
         <v>757</v>
       </c>
-      <c r="I31">
+      <c r="I32" s="11">
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
         <v>28273</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C32" t="s">
-        <v>727</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C33" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D33" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E32">
+      <c r="E33" s="11">
         <v>28273</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F33" s="11" t="s">
         <v>1008</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G33" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H33" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="I32">
+      <c r="I33" s="11">
         <v>97.409326424870471</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
         <v>29040</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E34" s="11" t="s">
         <v>1004</v>
       </c>
-      <c r="F33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" t="s">
+      <c r="F34" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H34" s="11" t="s">
         <v>1005</v>
       </c>
-      <c r="I33">
+      <c r="I34" s="11">
         <v>98.963730569948183</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="11">
         <v>29632</v>
       </c>
-      <c r="B34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="B35" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" s="11" t="s">
         <v>1006</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F35" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G35" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H35" s="11" t="s">
         <v>1007</v>
       </c>
-      <c r="I34">
+      <c r="I35" s="11">
         <v>99.481865284974091</v>
       </c>
     </row>
@@ -29876,6 +29967,369 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>2706</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>1011</v>
+      </c>
+      <c r="I2" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>3768</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>1013</v>
+      </c>
+      <c r="I3" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>9721</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>1014</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>1015</v>
+      </c>
+      <c r="I4" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>12514</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>1016</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>1017</v>
+      </c>
+      <c r="I5" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>12748</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>1019</v>
+      </c>
+      <c r="I6" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>13356</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>786</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>820</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>1021</v>
+      </c>
+      <c r="I7" s="11">
+        <v>78.899082568807344</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>17331</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>1023</v>
+      </c>
+      <c r="I8" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>19164</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>1024</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>1025</v>
+      </c>
+      <c r="I9" s="11">
+        <v>99.082568807339456</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>19955</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>1026</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>1027</v>
+      </c>
+      <c r="I10" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>21220</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>1029</v>
+      </c>
+      <c r="I11" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>25906</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>807</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>808</v>
+      </c>
+      <c r="I12" s="11">
+        <v>98.165137614678898</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>

</xml_diff>

<commit_message>
avoid mutation table NaN positions (and print to screen)
</commit_message>
<xml_diff>
--- a/mutationsTable.xlsx
+++ b/mutationsTable.xlsx
@@ -33765,8 +33765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changed order of variants
</commit_message>
<xml_diff>
--- a/mutationsTable.xlsx
+++ b/mutationsTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" tabRatio="846" firstSheet="8" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" tabRatio="846" firstSheet="8" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="B.1.1.7" sheetId="13" r:id="rId1"/>
@@ -26,12 +26,12 @@
     <sheet name="B.1.620" sheetId="11" r:id="rId12"/>
     <sheet name="AT.1" sheetId="12" r:id="rId13"/>
     <sheet name="B.1.617.1" sheetId="14" r:id="rId14"/>
-    <sheet name="B.1.617.2" sheetId="15" r:id="rId15"/>
-    <sheet name="B.1.617.2-a" sheetId="43" r:id="rId16"/>
-    <sheet name="B.1.617.2-b" sheetId="44" r:id="rId17"/>
-    <sheet name="B.1.617.2-c" sheetId="45" r:id="rId18"/>
-    <sheet name="B.1.617.2-d" sheetId="46" r:id="rId19"/>
-    <sheet name="B.1.617.2-e" sheetId="48" r:id="rId20"/>
+    <sheet name="B.1.617.2-a" sheetId="43" r:id="rId15"/>
+    <sheet name="B.1.617.2-b" sheetId="44" r:id="rId16"/>
+    <sheet name="B.1.617.2-c" sheetId="45" r:id="rId17"/>
+    <sheet name="B.1.617.2-d" sheetId="46" r:id="rId18"/>
+    <sheet name="B.1.617.2-e" sheetId="48" r:id="rId19"/>
+    <sheet name="B.1.617.2" sheetId="15" r:id="rId20"/>
     <sheet name="B.1.617.3" sheetId="16" r:id="rId21"/>
     <sheet name="C.37" sheetId="17" r:id="rId22"/>
     <sheet name="B.1.618" sheetId="18" r:id="rId23"/>
@@ -11289,967 +11289,6 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I40"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="56.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>210</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E2">
-        <v>210</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" t="s">
-        <v>488</v>
-      </c>
-      <c r="I2" s="1">
-        <v>99.775784753363226</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>15451</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" t="s">
-        <v>521</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" t="s">
-        <v>522</v>
-      </c>
-      <c r="I3" s="1">
-        <v>89.91031390134529</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>16466</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>177</v>
-      </c>
-      <c r="E4" t="s">
-        <v>347</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>179</v>
-      </c>
-      <c r="H4" t="s">
-        <v>348</v>
-      </c>
-      <c r="I4" s="1">
-        <v>89.013452914798208</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>21618</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>515</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>516</v>
-      </c>
-      <c r="I5" s="1">
-        <v>99.775784753363226</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>22029</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>727</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>523</v>
-      </c>
-      <c r="F6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>524</v>
-      </c>
-      <c r="I6" s="1">
-        <v>84.97757847533633</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>22030</v>
-      </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>727</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>523</v>
-      </c>
-      <c r="F7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>524</v>
-      </c>
-      <c r="I7" s="1">
-        <v>84.97757847533633</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>22031</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>727</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>523</v>
-      </c>
-      <c r="F8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" t="s">
-        <v>524</v>
-      </c>
-      <c r="I8" s="1">
-        <v>84.97757847533633</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>22032</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>727</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>523</v>
-      </c>
-      <c r="F9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" t="s">
-        <v>524</v>
-      </c>
-      <c r="I9" s="1">
-        <v>84.97757847533633</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>22033</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>727</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>523</v>
-      </c>
-      <c r="F10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" t="s">
-        <v>524</v>
-      </c>
-      <c r="I10" s="1">
-        <v>84.97757847533633</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>22034</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>727</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>523</v>
-      </c>
-      <c r="F11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" t="s">
-        <v>524</v>
-      </c>
-      <c r="I11" s="1">
-        <v>84.97757847533633</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>22917</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>89</v>
-      </c>
-      <c r="F12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" t="s">
-        <v>90</v>
-      </c>
-      <c r="I12" s="1">
-        <v>99.775784753363226</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>22995</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>517</v>
-      </c>
-      <c r="F13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" t="s">
-        <v>518</v>
-      </c>
-      <c r="I13" s="1">
-        <v>99.551569506726452</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>23604</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
-        <v>185</v>
-      </c>
-      <c r="F14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" t="s">
-        <v>186</v>
-      </c>
-      <c r="I14" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>24410</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" t="s">
-        <v>519</v>
-      </c>
-      <c r="F15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" t="s">
-        <v>520</v>
-      </c>
-      <c r="I15" s="1">
-        <v>88.340807174887885</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>25469</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" t="s">
-        <v>484</v>
-      </c>
-      <c r="F16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16" t="s">
-        <v>485</v>
-      </c>
-      <c r="I16" s="1">
-        <v>99.775784753363226</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>26767</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E17" t="s">
-        <v>303</v>
-      </c>
-      <c r="F17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" t="s">
-        <v>106</v>
-      </c>
-      <c r="H17" t="s">
-        <v>304</v>
-      </c>
-      <c r="I17" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>27638</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" t="s">
-        <v>486</v>
-      </c>
-      <c r="F18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H18" t="s">
-        <v>487</v>
-      </c>
-      <c r="I18" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>27752</v>
-      </c>
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" t="s">
-        <v>513</v>
-      </c>
-      <c r="F19" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" t="s">
-        <v>28</v>
-      </c>
-      <c r="H19" t="s">
-        <v>514</v>
-      </c>
-      <c r="I19" s="1">
-        <v>99.551569506726452</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>28248</v>
-      </c>
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" t="s">
-        <v>727</v>
-      </c>
-      <c r="D20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" t="s">
-        <v>359</v>
-      </c>
-      <c r="F20" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" t="s">
-        <v>73</v>
-      </c>
-      <c r="H20" t="s">
-        <v>360</v>
-      </c>
-      <c r="I20" s="1">
-        <v>78.25112107623319</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>28249</v>
-      </c>
-      <c r="B21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s">
-        <v>727</v>
-      </c>
-      <c r="D21" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" t="s">
-        <v>359</v>
-      </c>
-      <c r="F21" t="s">
-        <v>45</v>
-      </c>
-      <c r="G21" t="s">
-        <v>73</v>
-      </c>
-      <c r="H21" t="s">
-        <v>360</v>
-      </c>
-      <c r="I21" s="1">
-        <v>78.25112107623319</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>28250</v>
-      </c>
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" t="s">
-        <v>727</v>
-      </c>
-      <c r="D22" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" t="s">
-        <v>359</v>
-      </c>
-      <c r="F22" t="s">
-        <v>45</v>
-      </c>
-      <c r="G22" t="s">
-        <v>73</v>
-      </c>
-      <c r="H22" t="s">
-        <v>360</v>
-      </c>
-      <c r="I22" s="1">
-        <v>78.25112107623319</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>28251</v>
-      </c>
-      <c r="B23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" t="s">
-        <v>727</v>
-      </c>
-      <c r="D23" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" t="s">
-        <v>359</v>
-      </c>
-      <c r="F23" t="s">
-        <v>45</v>
-      </c>
-      <c r="G23" t="s">
-        <v>73</v>
-      </c>
-      <c r="H23" t="s">
-        <v>360</v>
-      </c>
-      <c r="I23" s="1">
-        <v>78.25112107623319</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>28252</v>
-      </c>
-      <c r="B24" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" t="s">
-        <v>727</v>
-      </c>
-      <c r="D24" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" t="s">
-        <v>359</v>
-      </c>
-      <c r="F24" t="s">
-        <v>45</v>
-      </c>
-      <c r="G24" t="s">
-        <v>73</v>
-      </c>
-      <c r="H24" t="s">
-        <v>360</v>
-      </c>
-      <c r="I24" s="1">
-        <v>78.25112107623319</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>28253</v>
-      </c>
-      <c r="B25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" t="s">
-        <v>727</v>
-      </c>
-      <c r="D25" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" t="s">
-        <v>359</v>
-      </c>
-      <c r="F25" t="s">
-        <v>45</v>
-      </c>
-      <c r="G25" t="s">
-        <v>73</v>
-      </c>
-      <c r="H25" t="s">
-        <v>360</v>
-      </c>
-      <c r="I25" s="1">
-        <v>78.25112107623319</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>28273</v>
-      </c>
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" t="s">
-        <v>727</v>
-      </c>
-      <c r="D26" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26">
-        <v>28273</v>
-      </c>
-      <c r="F26" t="s">
-        <v>1008</v>
-      </c>
-      <c r="G26" t="s">
-        <v>50</v>
-      </c>
-      <c r="H26" t="s">
-        <v>99</v>
-      </c>
-      <c r="I26" s="1">
-        <v>79.596412556053806</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>28461</v>
-      </c>
-      <c r="B27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" t="s">
-        <v>511</v>
-      </c>
-      <c r="F27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" t="s">
-        <v>22</v>
-      </c>
-      <c r="H27" t="s">
-        <v>512</v>
-      </c>
-      <c r="I27" s="1">
-        <v>95.964125560538122</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>28881</v>
-      </c>
-      <c r="B28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" t="s">
-        <v>482</v>
-      </c>
-      <c r="F28" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" t="s">
-        <v>483</v>
-      </c>
-      <c r="I28" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>29402</v>
-      </c>
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" t="s">
-        <v>489</v>
-      </c>
-      <c r="F29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" t="s">
-        <v>22</v>
-      </c>
-      <c r="H29" t="s">
-        <v>490</v>
-      </c>
-      <c r="I29" s="1">
-        <v>99.327354260089677</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29742</v>
-      </c>
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" t="s">
-        <v>48</v>
-      </c>
-      <c r="E30">
-        <v>29742</v>
-      </c>
-      <c r="F30" t="s">
-        <v>49</v>
-      </c>
-      <c r="G30" t="s">
-        <v>50</v>
-      </c>
-      <c r="H30" t="s">
-        <v>205</v>
-      </c>
-      <c r="I30" s="1">
-        <v>99.103139013452918</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31"/>
-    </row>
-    <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32"/>
-      <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32"/>
-      <c r="I32"/>
-    </row>
-    <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
-    </row>
-    <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
-      <c r="G34"/>
-      <c r="H34"/>
-      <c r="I34"/>
-    </row>
-    <row r="35" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35"/>
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="D35"/>
-      <c r="E35"/>
-      <c r="F35"/>
-      <c r="G35"/>
-      <c r="H35"/>
-      <c r="I35"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F36" s="6"/>
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I40" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13365,7 +12404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
@@ -14482,7 +13521,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
@@ -15715,7 +14754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I42"/>
   <sheetViews>
@@ -16941,6 +15980,949 @@
       </c>
       <c r="I42" s="11">
         <v>98.950131233595798</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>210</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="6">
+        <v>210</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="I2" s="6">
+        <v>98.760330578512395</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>1191</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>1120</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>1121</v>
+      </c>
+      <c r="I3" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>1267</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>1122</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>1123</v>
+      </c>
+      <c r="I4" s="6">
+        <v>99.586776859504127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>5184</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>847</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>848</v>
+      </c>
+      <c r="I5" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>9203</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>709</v>
+      </c>
+      <c r="I6" s="6">
+        <v>99.586776859504127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>9678</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>1152</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>1155</v>
+      </c>
+      <c r="I7" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>11005</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>889</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>890</v>
+      </c>
+      <c r="I8" s="6">
+        <v>88.429752066115711</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>17496</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>1156</v>
+      </c>
+      <c r="I9" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>20396</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="I10" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>21618</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>516</v>
+      </c>
+      <c r="I11" s="6">
+        <v>99.586776859504127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>21792</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>1154</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>1157</v>
+      </c>
+      <c r="I12" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>22029</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="I13" s="6">
+        <v>84.297520661157023</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>22030</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="I14" s="6">
+        <v>84.297520661157023</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>22031</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="I15" s="6">
+        <v>84.297520661157023</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>22032</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="I16" s="6">
+        <v>84.297520661157023</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>22033</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="I17" s="6">
+        <v>84.297520661157023</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>22034</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="I18" s="6">
+        <v>84.297520661157023</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>22917</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I19" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>22995</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="I20" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>23604</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="I21" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>24410</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="I22" s="6">
+        <v>84.710743801652882</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>25469</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="I23" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>26767</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="I24" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>27638</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="I25" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>27752</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="I26" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>28253</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="I27" s="6">
+        <v>95.041322314049594</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>28273</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="6">
+        <v>28273</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>1007</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I28" s="6">
+        <v>78.925619834710744</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>28461</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="I29" s="6">
+        <v>93.801652892561975</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>28881</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="I30" s="6">
+        <v>98.347107438016536</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>29402</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="I31" s="6">
+        <v>99.586776859504127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>29742</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="6">
+        <v>29742</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="I32" s="6">
+        <v>87.603305785123965</v>
       </c>
     </row>
   </sheetData>
@@ -18247,941 +18229,959 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2">
         <v>210</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>212</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2">
         <v>210</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" t="s">
         <v>488</v>
       </c>
-      <c r="I2" s="6">
-        <v>98.760330578512395</v>
+      <c r="I2" s="1">
+        <v>99.775784753363226</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>1191</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>1121</v>
-      </c>
-      <c r="I3" s="6">
+      <c r="A3">
+        <v>15451</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>521</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>522</v>
+      </c>
+      <c r="I3" s="1">
+        <v>89.91031390134529</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>16466</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E4" t="s">
+        <v>347</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>179</v>
+      </c>
+      <c r="H4" t="s">
+        <v>348</v>
+      </c>
+      <c r="I4" s="1">
+        <v>89.013452914798208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>21618</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>515</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>516</v>
+      </c>
+      <c r="I5" s="1">
+        <v>99.775784753363226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>22029</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>727</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>523</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>524</v>
+      </c>
+      <c r="I6" s="1">
+        <v>84.97757847533633</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>22030</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>727</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>523</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>524</v>
+      </c>
+      <c r="I7" s="1">
+        <v>84.97757847533633</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>22031</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>727</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>523</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>524</v>
+      </c>
+      <c r="I8" s="1">
+        <v>84.97757847533633</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>22032</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>727</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>523</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>524</v>
+      </c>
+      <c r="I9" s="1">
+        <v>84.97757847533633</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>22033</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>727</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>523</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>524</v>
+      </c>
+      <c r="I10" s="1">
+        <v>84.97757847533633</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>22034</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>523</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" t="s">
+        <v>524</v>
+      </c>
+      <c r="I11" s="1">
+        <v>84.97757847533633</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>22917</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="1">
+        <v>99.775784753363226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>22995</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>517</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>518</v>
+      </c>
+      <c r="I13" s="1">
+        <v>99.551569506726452</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>23604</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>185</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>186</v>
+      </c>
+      <c r="I14" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>1267</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>1122</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>1123</v>
-      </c>
-      <c r="I4" s="6">
-        <v>99.586776859504127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>5184</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>847</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>848</v>
-      </c>
-      <c r="I5" s="6">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>24410</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>519</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>520</v>
+      </c>
+      <c r="I15" s="1">
+        <v>88.340807174887885</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>25469</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
+        <v>484</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" t="s">
+        <v>485</v>
+      </c>
+      <c r="I16" s="1">
+        <v>99.775784753363226</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>26767</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" t="s">
+        <v>303</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" t="s">
+        <v>106</v>
+      </c>
+      <c r="H17" t="s">
+        <v>304</v>
+      </c>
+      <c r="I17" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>9203</v>
-      </c>
-      <c r="B6" s="6" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>27638</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" t="s">
+        <v>486</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" t="s">
+        <v>487</v>
+      </c>
+      <c r="I18" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>27752</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s">
+        <v>513</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" t="s">
+        <v>514</v>
+      </c>
+      <c r="I19" s="1">
+        <v>99.551569506726452</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>28248</v>
+      </c>
+      <c r="B20" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C20" t="s">
+        <v>727</v>
+      </c>
+      <c r="D20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" t="s">
+        <v>359</v>
+      </c>
+      <c r="F20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" t="s">
+        <v>360</v>
+      </c>
+      <c r="I20" s="1">
+        <v>78.25112107623319</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>28249</v>
+      </c>
+      <c r="B21" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>708</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>709</v>
-      </c>
-      <c r="I6" s="6">
-        <v>99.586776859504127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>9678</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>1152</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>1155</v>
-      </c>
-      <c r="I7" s="6">
+      <c r="C21" t="s">
+        <v>727</v>
+      </c>
+      <c r="D21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" t="s">
+        <v>359</v>
+      </c>
+      <c r="F21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" t="s">
+        <v>360</v>
+      </c>
+      <c r="I21" s="1">
+        <v>78.25112107623319</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>28250</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>727</v>
+      </c>
+      <c r="D22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" t="s">
+        <v>359</v>
+      </c>
+      <c r="F22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" t="s">
+        <v>360</v>
+      </c>
+      <c r="I22" s="1">
+        <v>78.25112107623319</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>28251</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>727</v>
+      </c>
+      <c r="D23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" t="s">
+        <v>359</v>
+      </c>
+      <c r="F23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" t="s">
+        <v>73</v>
+      </c>
+      <c r="H23" t="s">
+        <v>360</v>
+      </c>
+      <c r="I23" s="1">
+        <v>78.25112107623319</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>28252</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>727</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" t="s">
+        <v>359</v>
+      </c>
+      <c r="F24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24" t="s">
+        <v>73</v>
+      </c>
+      <c r="H24" t="s">
+        <v>360</v>
+      </c>
+      <c r="I24" s="1">
+        <v>78.25112107623319</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>28253</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>727</v>
+      </c>
+      <c r="D25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" t="s">
+        <v>359</v>
+      </c>
+      <c r="F25" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" t="s">
+        <v>360</v>
+      </c>
+      <c r="I25" s="1">
+        <v>78.25112107623319</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>28273</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>727</v>
+      </c>
+      <c r="D26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26">
+        <v>28273</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1008</v>
+      </c>
+      <c r="G26" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" t="s">
+        <v>99</v>
+      </c>
+      <c r="I26" s="1">
+        <v>79.596412556053806</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>28461</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" t="s">
+        <v>511</v>
+      </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" t="s">
+        <v>512</v>
+      </c>
+      <c r="I27" s="1">
+        <v>95.964125560538122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28881</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" t="s">
+        <v>482</v>
+      </c>
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" t="s">
+        <v>483</v>
+      </c>
+      <c r="I28" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>11005</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>889</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>890</v>
-      </c>
-      <c r="I8" s="6">
-        <v>88.429752066115711</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>17496</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="6" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29402</v>
+      </c>
+      <c r="B29" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>1153</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>1156</v>
-      </c>
-      <c r="I9" s="6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>20396</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" t="s">
+        <v>489</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" t="s">
+        <v>490</v>
+      </c>
+      <c r="I29" s="1">
+        <v>99.327354260089677</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29742</v>
+      </c>
+      <c r="B30" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>493</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>494</v>
-      </c>
-      <c r="I10" s="6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>21618</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>515</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>516</v>
-      </c>
-      <c r="I11" s="6">
-        <v>99.586776859504127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>21792</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>1154</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>1157</v>
-      </c>
-      <c r="I12" s="6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>22029</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>727</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>523</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>524</v>
-      </c>
-      <c r="I13" s="6">
-        <v>84.297520661157023</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>22030</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>727</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>523</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>524</v>
-      </c>
-      <c r="I14" s="6">
-        <v>84.297520661157023</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>22031</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>727</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>523</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>524</v>
-      </c>
-      <c r="I15" s="6">
-        <v>84.297520661157023</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <v>22032</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>727</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>523</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>524</v>
-      </c>
-      <c r="I16" s="6">
-        <v>84.297520661157023</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>22033</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>727</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>523</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>524</v>
-      </c>
-      <c r="I17" s="6">
-        <v>84.297520661157023</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>22034</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>727</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>523</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>524</v>
-      </c>
-      <c r="I18" s="6">
-        <v>84.297520661157023</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>22917</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="I19" s="6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <v>22995</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>517</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>518</v>
-      </c>
-      <c r="I20" s="6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>23604</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="I21" s="6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <v>24410</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>519</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>520</v>
-      </c>
-      <c r="I22" s="6">
-        <v>84.710743801652882</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
-        <v>25469</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>484</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>485</v>
-      </c>
-      <c r="I23" s="6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <v>26767</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="I24" s="6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
-        <v>27638</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>486</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>487</v>
-      </c>
-      <c r="I25" s="6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
-        <v>27752</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>513</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>514</v>
-      </c>
-      <c r="I26" s="6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
-        <v>28253</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="I27" s="6">
-        <v>95.041322314049594</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
-        <v>28273</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>727</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="6">
-        <v>28273</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>1007</v>
-      </c>
-      <c r="G28" s="6" t="s">
+      <c r="E30">
+        <v>29742</v>
+      </c>
+      <c r="F30" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" t="s">
         <v>50</v>
       </c>
-      <c r="H28" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="I28" s="6">
-        <v>78.925619834710744</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
-        <v>28461</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>511</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>512</v>
-      </c>
-      <c r="I29" s="6">
-        <v>93.801652892561975</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
-        <v>28881</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>482</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="I30" s="6">
-        <v>98.347107438016536</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
-        <v>29402</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>489</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="I31" s="6">
-        <v>99.586776859504127</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
-        <v>29742</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E32" s="6">
-        <v>29742</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H32" s="6" t="s">
+      <c r="H30" t="s">
         <v>205</v>
       </c>
-      <c r="I32" s="6">
-        <v>87.603305785123965</v>
-      </c>
+      <c r="I30" s="1">
+        <v>99.103139013452918</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+    </row>
+    <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+    </row>
+    <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+    </row>
+    <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+    </row>
+    <row r="35" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F36" s="6"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19770,7 +19770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated mutations table : added AY.1 AY.3
</commit_message>
<xml_diff>
--- a/mutationsTable.xlsx
+++ b/mutationsTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" tabRatio="846" firstSheet="8" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" tabRatio="846" firstSheet="26" activeTab="45"/>
   </bookViews>
   <sheets>
     <sheet name="B.1.1.7" sheetId="13" r:id="rId1"/>
@@ -55,11 +55,13 @@
     <sheet name="A.29" sheetId="35" r:id="rId41"/>
     <sheet name="AW.1" sheetId="38" r:id="rId42"/>
     <sheet name="B.1.1.523" sheetId="39" r:id="rId43"/>
-    <sheet name="AY.2" sheetId="40" r:id="rId44"/>
-    <sheet name="B.1.626" sheetId="41" r:id="rId45"/>
-    <sheet name="B.1.627" sheetId="49" r:id="rId46"/>
-    <sheet name="B.1.628" sheetId="50" r:id="rId47"/>
-    <sheet name="B.1.629" sheetId="51" r:id="rId48"/>
+    <sheet name="AY.1" sheetId="52" r:id="rId44"/>
+    <sheet name="AY.2" sheetId="40" r:id="rId45"/>
+    <sheet name="AY.3" sheetId="53" r:id="rId46"/>
+    <sheet name="B.1.626" sheetId="41" r:id="rId47"/>
+    <sheet name="B.1.627" sheetId="49" r:id="rId48"/>
+    <sheet name="B.1.628" sheetId="50" r:id="rId49"/>
+    <sheet name="B.1.629" sheetId="51" r:id="rId50"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -71,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10453" uniqueCount="1249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11061" uniqueCount="1257">
   <si>
     <t>Position</t>
   </si>
@@ -3818,6 +3820,30 @@
   </si>
   <si>
     <t>S:K182R</t>
+  </si>
+  <si>
+    <t>W258L</t>
+  </si>
+  <si>
+    <t>S:W258L</t>
+  </si>
+  <si>
+    <t>I162V</t>
+  </si>
+  <si>
+    <t>NSP6:I162V</t>
+  </si>
+  <si>
+    <t>R259R</t>
+  </si>
+  <si>
+    <t>N:R259R</t>
+  </si>
+  <si>
+    <t>S412S</t>
+  </si>
+  <si>
+    <t>N:S412S</t>
   </si>
 </sst>
 </file>
@@ -18231,7 +18257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
@@ -38481,10 +38507,1301 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>210</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="11">
+        <v>210</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="I2" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>4181</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>1139</v>
+      </c>
+      <c r="I3" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>6402</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>1141</v>
+      </c>
+      <c r="I4" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>7124</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>559</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>560</v>
+      </c>
+      <c r="I5" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>8986</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>1143</v>
+      </c>
+      <c r="I6" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>9053</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>1145</v>
+      </c>
+      <c r="I7" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>10029</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>427</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>428</v>
+      </c>
+      <c r="I8" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>11201</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>491</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>492</v>
+      </c>
+      <c r="I9" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>11332</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>1147</v>
+      </c>
+      <c r="I10" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>15451</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>521</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="I11" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>16466</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="I12" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>19220</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>1149</v>
+      </c>
+      <c r="I13" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>21618</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>515</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>516</v>
+      </c>
+      <c r="I14" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>21846</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="I15" s="11">
+        <v>92.361111111111114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>22029</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="I16" s="11">
+        <v>90.277777777777786</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>22030</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="I17" s="11">
+        <v>90.277777777777786</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>22031</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="I18" s="11">
+        <v>90.277777777777786</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>22032</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="I19" s="11">
+        <v>90.277777777777786</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
+        <v>22033</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="I20" s="11">
+        <v>90.277777777777786</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>22034</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="I21" s="11">
+        <v>90.277777777777786</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>22335</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>1249</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>1250</v>
+      </c>
+      <c r="I22" s="11">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>22813</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I23" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <v>22917</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I24" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>22995</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>517</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>518</v>
+      </c>
+      <c r="I25" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
+        <v>23604</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="I26" s="11">
+        <v>99.305555555555557</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
+        <v>24410</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>519</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="I27" s="11">
+        <v>94.444444444444443</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
+        <v>25469</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>484</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="I28" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
+        <v>26767</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="I29" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
+        <v>27638</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>486</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="I30" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
+        <v>27752</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>513</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>514</v>
+      </c>
+      <c r="I31" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
+        <v>27874</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>399</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>1150</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>401</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>1151</v>
+      </c>
+      <c r="I32" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
+        <v>28248</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="I33" s="11">
+        <v>94.444444444444443</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
+        <v>28249</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="I34" s="11">
+        <v>94.444444444444443</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11">
+        <v>28250</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="I35" s="11">
+        <v>94.444444444444443</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11">
+        <v>28251</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="I36" s="11">
+        <v>94.444444444444443</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
+        <v>28252</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="I37" s="11">
+        <v>94.444444444444443</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
+        <v>28253</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="I38" s="11">
+        <v>94.444444444444443</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="11">
+        <v>28273</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E39" s="11">
+        <v>28273</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>1008</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I39" s="11">
+        <v>92.361111111111114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="11">
+        <v>28461</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>511</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>512</v>
+      </c>
+      <c r="I40" s="11">
+        <v>98.611111111111114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="11">
+        <v>28881</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>482</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>483</v>
+      </c>
+      <c r="I41" s="11">
+        <v>99.305555555555557</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="11">
+        <v>28916</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>867</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>868</v>
+      </c>
+      <c r="I42" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="11">
+        <v>29402</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>489</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>490</v>
+      </c>
+      <c r="I43" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="11">
+        <v>29742</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E44" s="11">
+        <v>29742</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H44" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="I44" s="11">
+        <v>99.305555555555557</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39799,12 +41116,1274 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>210</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="11">
+        <v>210</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="I2" s="11">
+        <v>99.280575539568346</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>4181</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>1139</v>
+      </c>
+      <c r="I3" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>6402</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>1141</v>
+      </c>
+      <c r="I4" s="11">
+        <v>99.280575539568346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>7124</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>559</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>560</v>
+      </c>
+      <c r="I5" s="11">
+        <v>99.280575539568346</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>8986</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>1143</v>
+      </c>
+      <c r="I6" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>9053</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>1145</v>
+      </c>
+      <c r="I7" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>10029</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>427</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>428</v>
+      </c>
+      <c r="I8" s="11">
+        <v>99.280575539568346</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>11201</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>491</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>492</v>
+      </c>
+      <c r="I9" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>11332</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>1147</v>
+      </c>
+      <c r="I10" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>11456</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>1251</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>1252</v>
+      </c>
+      <c r="I11" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>15451</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>521</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="I12" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>16466</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="I13" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>19220</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>1149</v>
+      </c>
+      <c r="I14" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>21618</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>515</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>516</v>
+      </c>
+      <c r="I15" s="11">
+        <v>99.280575539568346</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>22029</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="I16" s="11">
+        <v>94.964028776978409</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>22030</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="I17" s="11">
+        <v>94.964028776978409</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>22031</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="I18" s="11">
+        <v>94.964028776978409</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>22032</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="I19" s="11">
+        <v>94.964028776978409</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
+        <v>22033</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="I20" s="11">
+        <v>94.964028776978409</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>22034</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="I21" s="11">
+        <v>94.964028776978409</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>22917</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I22" s="11">
+        <v>98.561151079136692</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>22995</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>517</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>518</v>
+      </c>
+      <c r="I23" s="11">
+        <v>98.561151079136692</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <v>23604</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="I24" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>24410</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>519</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="I25" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
+        <v>25469</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>484</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="I26" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
+        <v>26767</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="I27" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
+        <v>27638</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>486</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="I28" s="11">
+        <v>98.561151079136692</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
+        <v>27752</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>513</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>514</v>
+      </c>
+      <c r="I29" s="11">
+        <v>98.561151079136692</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
+        <v>27874</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>399</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>1150</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>401</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>1151</v>
+      </c>
+      <c r="I30" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
+        <v>28248</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="I31" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
+        <v>28249</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="I32" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
+        <v>28250</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="I33" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
+        <v>28251</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="I34" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11">
+        <v>28252</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="I35" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11">
+        <v>28253</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="I36" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
+        <v>28273</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" s="11">
+        <v>28273</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>1008</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I37" s="11">
+        <v>95.683453237410077</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
+        <v>28461</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>511</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>512</v>
+      </c>
+      <c r="I38" s="11">
+        <v>99.280575539568346</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="11">
+        <v>28881</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>482</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>483</v>
+      </c>
+      <c r="I39" s="11">
+        <v>92.086330935251809</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="11">
+        <v>28916</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>867</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>868</v>
+      </c>
+      <c r="I40" s="11">
+        <v>92.086330935251809</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="11">
+        <v>29050</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>1253</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>1254</v>
+      </c>
+      <c r="I41" s="11">
+        <v>98.561151079136692</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="11">
+        <v>29402</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>489</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>490</v>
+      </c>
+      <c r="I42" s="11">
+        <v>99.280575539568346</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="11">
+        <v>29509</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>1255</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>1256</v>
+      </c>
+      <c r="I43" s="11">
+        <v>99.280575539568346</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40977,12 +43556,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41949,7 +44528,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
@@ -43146,780 +45725,6 @@
       </c>
       <c r="I41" s="1">
         <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="56.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
-        <v>815</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>1220</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>1221</v>
-      </c>
-      <c r="I2" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
-        <v>1191</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>1120</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>1121</v>
-      </c>
-      <c r="I3" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
-        <v>2416</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>1222</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>1223</v>
-      </c>
-      <c r="I4" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
-        <v>3040</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>1224</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>1225</v>
-      </c>
-      <c r="I5" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
-        <v>4229</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>1226</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>1227</v>
-      </c>
-      <c r="I6" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
-        <v>5095</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>1228</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>1229</v>
-      </c>
-      <c r="I7" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
-        <v>5178</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="I8" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
-        <v>11128</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>1230</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>1231</v>
-      </c>
-      <c r="I9" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
-        <v>12459</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>1232</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>1233</v>
-      </c>
-      <c r="I10" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
-        <v>14322</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>1234</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>1235</v>
-      </c>
-      <c r="I11" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
-        <v>21987</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>507</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>508</v>
-      </c>
-      <c r="I12" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
-        <v>22917</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="I13" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
-        <v>22995</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>517</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>518</v>
-      </c>
-      <c r="I14" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
-        <v>23948</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>353</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>354</v>
-      </c>
-      <c r="I15" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
-        <v>25563</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="I16" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
-        <v>26038</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>1236</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>1237</v>
-      </c>
-      <c r="I17" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
-        <v>26498</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="11">
-        <v>26498</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>1061</v>
-      </c>
-      <c r="I18" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
-        <v>26767</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>987</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>988</v>
-      </c>
-      <c r="I19" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
-        <v>28482</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>1238</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>1239</v>
-      </c>
-      <c r="I20" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
-        <v>23604</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>384</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>385</v>
-      </c>
-      <c r="I21" s="1">
-        <v>97.435897435897431</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
-        <v>25433</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>637</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>1240</v>
-      </c>
-      <c r="I22" s="1">
-        <v>97.435897435897431</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
-        <v>25266</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>1241</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>1242</v>
-      </c>
-      <c r="I23" s="1">
-        <v>89.743589743589752</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
-        <v>28833</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>1243</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>1244</v>
-      </c>
-      <c r="I24" s="1">
-        <v>89.743589743589752</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
-        <v>28926</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>1245</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>1246</v>
-      </c>
-      <c r="I25" s="1">
-        <v>89.743589743589752</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
-        <v>22107</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>1247</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>1248</v>
-      </c>
-      <c r="I26" s="1">
-        <v>87.179487179487182</v>
       </c>
     </row>
   </sheetData>
@@ -45801,6 +47606,780 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>815</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>1220</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>1221</v>
+      </c>
+      <c r="I2" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>1191</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>1120</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>1121</v>
+      </c>
+      <c r="I3" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>2416</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>1222</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>1223</v>
+      </c>
+      <c r="I4" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>3040</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>1225</v>
+      </c>
+      <c r="I5" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>4229</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>1227</v>
+      </c>
+      <c r="I6" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>5095</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>1228</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>1229</v>
+      </c>
+      <c r="I7" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>5178</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="I8" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>11128</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>1230</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>1231</v>
+      </c>
+      <c r="I9" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>12459</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>1232</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>1233</v>
+      </c>
+      <c r="I10" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>14322</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>1234</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>1235</v>
+      </c>
+      <c r="I11" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>21987</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>507</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>508</v>
+      </c>
+      <c r="I12" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>22917</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>22995</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>517</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>518</v>
+      </c>
+      <c r="I14" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>23948</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="I15" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>25563</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>26038</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>1236</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>1237</v>
+      </c>
+      <c r="I17" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>26498</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="11">
+        <v>26498</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>1061</v>
+      </c>
+      <c r="I18" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>26767</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>987</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>988</v>
+      </c>
+      <c r="I19" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
+        <v>28482</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>1239</v>
+      </c>
+      <c r="I20" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>23604</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="I21" s="1">
+        <v>97.435897435897431</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>25433</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>637</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>1240</v>
+      </c>
+      <c r="I22" s="1">
+        <v>97.435897435897431</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>25266</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>1241</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>1242</v>
+      </c>
+      <c r="I23" s="1">
+        <v>89.743589743589752</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <v>28833</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>1243</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>1244</v>
+      </c>
+      <c r="I24" s="1">
+        <v>89.743589743589752</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>28926</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>1245</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>1246</v>
+      </c>
+      <c r="I25" s="1">
+        <v>89.743589743589752</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
+        <v>22107</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>1247</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>1248</v>
+      </c>
+      <c r="I26" s="1">
+        <v>87.179487179487182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>

</xml_diff>